<commit_message>
nettoyage codes + variables env + update maj bdd
</commit_message>
<xml_diff>
--- a/database/export.xlsx
+++ b/database/export.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xtian\OneDrive\Documents\CentralSupelec\projet\msdocs-flask-postgresql-sample-app\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F22C1515-ED4D-4BE9-BC38-16F4CF7AB8FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BAC5384-3424-4528-A209-EE17133C334A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1665" yWindow="735" windowWidth="20910" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>id_article</t>
   </si>
@@ -40,10 +40,7 @@
     <t>carbone_unite</t>
   </si>
   <si>
-    <t>name_1</t>
-  </si>
-  <si>
-    <t>name_3</t>
+    <t>name_5</t>
   </si>
 </sst>
 </file>
@@ -445,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,7 +475,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -490,23 +487,6 @@
         <v>999</v>
       </c>
       <c r="F2">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3">
-        <v>999</v>
-      </c>
-      <c r="F3">
         <v>999</v>
       </c>
     </row>

</xml_diff>

<commit_message>
resolu: gestion des problemes de timeout de l'update des fichiers excel
</commit_message>
<xml_diff>
--- a/database/export.xlsx
+++ b/database/export.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xtian\OneDrive\Documents\CentralSupelec\projet\msdocs-flask-postgresql-sample-app\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BAC5384-3424-4528-A209-EE17133C334A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C245FC6B-C3CA-4DB8-8366-4066C91D09AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1665" yWindow="735" windowWidth="20910" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4425" yWindow="3495" windowWidth="20910" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>id_article</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>name_5</t>
+  </si>
+  <si>
+    <t>Bug</t>
   </si>
 </sst>
 </file>
@@ -72,7 +75,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -95,13 +98,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -442,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,7 +470,7 @@
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -472,10 +489,13 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -487,7 +507,7 @@
         <v>999</v>
       </c>
       <c r="F2">
-        <v>999</v>
+        <v>9999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>